<commit_message>
added fetching tag id from name
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E86"/>
+  <dimension ref="A1:E88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -481,7 +481,7 @@
         <v>0.86</v>
       </c>
       <c r="C2" s="3" t="n">
-        <v>116032</v>
+        <v>116038</v>
       </c>
       <c r="D2" s="4" t="n">
         <v>3.99</v>
@@ -500,7 +500,7 @@
         <v>0.89</v>
       </c>
       <c r="C3" s="3" t="n">
-        <v>422685</v>
+        <v>422691</v>
       </c>
       <c r="D3" s="4" t="n">
         <v>0.99</v>
@@ -519,7 +519,7 @@
         <v>0.97</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>608245</v>
+        <v>608262</v>
       </c>
       <c r="D4" s="4" t="n">
         <v>0.97</v>
@@ -557,7 +557,7 @@
         <v>0.9</v>
       </c>
       <c r="C6" s="3" t="n">
-        <v>30551</v>
+        <v>30552</v>
       </c>
       <c r="D6" s="4" t="n">
         <v>2.99</v>
@@ -576,7 +576,7 @@
         <v>0.98</v>
       </c>
       <c r="C7" s="3" t="n">
-        <v>306852</v>
+        <v>306860</v>
       </c>
       <c r="D7" s="4" t="n">
         <v>0.97</v>
@@ -595,7 +595,7 @@
         <v>0.85</v>
       </c>
       <c r="C8" s="3" t="n">
-        <v>98580</v>
+        <v>98582</v>
       </c>
       <c r="D8" s="4" t="n">
         <v>8.99</v>
@@ -614,7 +614,7 @@
         <v>0.8</v>
       </c>
       <c r="C9" s="3" t="n">
-        <v>134880</v>
+        <v>134882</v>
       </c>
       <c r="D9" s="4" t="n">
         <v>8.99</v>
@@ -626,17 +626,17 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>STAR WARS™ Battlefront™ II</t>
+          <t>Titanfall® 2</t>
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>0.87</v>
+        <v>0.95</v>
       </c>
       <c r="C10" s="3" t="n">
-        <v>45033</v>
+        <v>177672</v>
       </c>
       <c r="D10" s="4" t="n">
-        <v>5.99</v>
+        <v>4.49</v>
       </c>
       <c r="E10" s="2" t="n">
         <v>0.85</v>
@@ -645,17 +645,17 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>Titanfall® 2</t>
+          <t>STAR WARS™ Battlefront™ II</t>
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>0.95</v>
+        <v>0.87</v>
       </c>
       <c r="C11" s="3" t="n">
-        <v>177667</v>
+        <v>45036</v>
       </c>
       <c r="D11" s="4" t="n">
-        <v>4.49</v>
+        <v>5.99</v>
       </c>
       <c r="E11" s="2" t="n">
         <v>0.85</v>
@@ -671,7 +671,7 @@
         <v>0.84</v>
       </c>
       <c r="C12" s="3" t="n">
-        <v>8036</v>
+        <v>8037</v>
       </c>
       <c r="D12" s="4" t="n">
         <v>5.99</v>
@@ -702,55 +702,55 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>Trailmakers</t>
+          <t>The Talos Principle</t>
         </is>
       </c>
       <c r="B14" s="2" t="n">
-        <v>0.93</v>
+        <v>0.95</v>
       </c>
       <c r="C14" s="3" t="n">
-        <v>16352</v>
+        <v>25376</v>
       </c>
       <c r="D14" s="4" t="n">
-        <v>6.06</v>
+        <v>4.34</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>0.82</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>Metro Exodus</t>
+          <t>Trailmakers</t>
         </is>
       </c>
       <c r="B15" s="2" t="n">
-        <v>0.89</v>
+        <v>0.93</v>
       </c>
       <c r="C15" s="3" t="n">
-        <v>86272</v>
+        <v>16355</v>
       </c>
       <c r="D15" s="4" t="n">
-        <v>5.99</v>
+        <v>6.06</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>0.8</v>
+        <v>0.82</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>DOOM</t>
+          <t>Metro Exodus</t>
         </is>
       </c>
       <c r="B16" s="2" t="n">
-        <v>0.95</v>
+        <v>0.89</v>
       </c>
       <c r="C16" s="3" t="n">
-        <v>124046</v>
+        <v>86275</v>
       </c>
       <c r="D16" s="4" t="n">
-        <v>3.99</v>
+        <v>5.99</v>
       </c>
       <c r="E16" s="2" t="n">
         <v>0.8</v>
@@ -759,17 +759,17 @@
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>Far Cry® 4</t>
+          <t>DOOM</t>
         </is>
       </c>
       <c r="B17" s="2" t="n">
-        <v>0.83</v>
+        <v>0.95</v>
       </c>
       <c r="C17" s="3" t="n">
-        <v>46101</v>
+        <v>124049</v>
       </c>
       <c r="D17" s="4" t="n">
-        <v>5.99</v>
+        <v>3.99</v>
       </c>
       <c r="E17" s="2" t="n">
         <v>0.8</v>
@@ -778,17 +778,17 @@
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>Unravel Two</t>
+          <t>Far Cry® 4</t>
         </is>
       </c>
       <c r="B18" s="2" t="n">
-        <v>0.82</v>
+        <v>0.83</v>
       </c>
       <c r="C18" s="3" t="n">
-        <v>4318</v>
+        <v>46101</v>
       </c>
       <c r="D18" s="4" t="n">
-        <v>3.99</v>
+        <v>5.99</v>
       </c>
       <c r="E18" s="2" t="n">
         <v>0.8</v>
@@ -804,7 +804,7 @@
         <v>0.95</v>
       </c>
       <c r="C19" s="3" t="n">
-        <v>99536</v>
+        <v>99537</v>
       </c>
       <c r="D19" s="4" t="n">
         <v>2.99</v>
@@ -816,33 +816,33 @@
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>It Takes Two</t>
+          <t>Unravel Two</t>
         </is>
       </c>
       <c r="B20" s="2" t="n">
-        <v>0.95</v>
+        <v>0.82</v>
       </c>
       <c r="C20" s="3" t="n">
-        <v>126946</v>
+        <v>4318</v>
       </c>
       <c r="D20" s="4" t="n">
-        <v>9.99</v>
+        <v>3.99</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>Halo: The Master Chief Collection</t>
+          <t>It Takes Two</t>
         </is>
       </c>
       <c r="B21" s="2" t="n">
-        <v>0.92</v>
+        <v>0.95</v>
       </c>
       <c r="C21" s="3" t="n">
-        <v>198198</v>
+        <v>126957</v>
       </c>
       <c r="D21" s="4" t="n">
         <v>9.99</v>
@@ -854,14 +854,14 @@
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>DOOM Eternal</t>
+          <t>Halo: The Master Chief Collection</t>
         </is>
       </c>
       <c r="B22" s="2" t="n">
-        <v>0.91</v>
+        <v>0.92</v>
       </c>
       <c r="C22" s="3" t="n">
-        <v>156949</v>
+        <v>198201</v>
       </c>
       <c r="D22" s="4" t="n">
         <v>9.99</v>
@@ -873,17 +873,17 @@
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>Celeste</t>
+          <t>DOOM Eternal</t>
         </is>
       </c>
       <c r="B23" s="2" t="n">
-        <v>0.97</v>
+        <v>0.91</v>
       </c>
       <c r="C23" s="3" t="n">
-        <v>77600</v>
+        <v>156951</v>
       </c>
       <c r="D23" s="4" t="n">
-        <v>4.99</v>
+        <v>9.99</v>
       </c>
       <c r="E23" s="2" t="n">
         <v>0.75</v>
@@ -892,17 +892,17 @@
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>Borderlands 2</t>
+          <t>Celeste</t>
         </is>
       </c>
       <c r="B24" s="2" t="n">
-        <v>0.95</v>
+        <v>0.97</v>
       </c>
       <c r="C24" s="3" t="n">
-        <v>186184</v>
+        <v>77605</v>
       </c>
       <c r="D24" s="4" t="n">
-        <v>7.49</v>
+        <v>4.99</v>
       </c>
       <c r="E24" s="2" t="n">
         <v>0.75</v>
@@ -911,17 +911,17 @@
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>Little Nightmares</t>
+          <t>Borderlands 2</t>
         </is>
       </c>
       <c r="B25" s="2" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.95</v>
       </c>
       <c r="C25" s="3" t="n">
-        <v>39402</v>
+        <v>186186</v>
       </c>
       <c r="D25" s="4" t="n">
-        <v>4.99</v>
+        <v>7.49</v>
       </c>
       <c r="E25" s="2" t="n">
         <v>0.75</v>
@@ -930,55 +930,55 @@
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>Inscryption</t>
+          <t>Little Nightmares</t>
         </is>
       </c>
       <c r="B26" s="2" t="n">
-        <v>0.96</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="C26" s="3" t="n">
-        <v>95550</v>
+        <v>39406</v>
       </c>
       <c r="D26" s="4" t="n">
-        <v>9.890000000000001</v>
+        <v>4.99</v>
       </c>
       <c r="E26" s="2" t="n">
-        <v>0.7</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>Keep Talking and Nobody Explodes</t>
+          <t>BioShock Infinite</t>
         </is>
       </c>
       <c r="B27" s="2" t="n">
-        <v>0.97</v>
+        <v>0.93</v>
       </c>
       <c r="C27" s="3" t="n">
-        <v>10784</v>
+        <v>100494</v>
       </c>
       <c r="D27" s="4" t="n">
-        <v>4.43</v>
+        <v>7.49</v>
       </c>
       <c r="E27" s="2" t="n">
-        <v>0.7</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>Human Fall Flat</t>
+          <t>Inscryption</t>
         </is>
       </c>
       <c r="B28" s="2" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.96</v>
       </c>
       <c r="C28" s="3" t="n">
-        <v>149817</v>
+        <v>95560</v>
       </c>
       <c r="D28" s="4" t="n">
-        <v>5.99</v>
+        <v>9.890000000000001</v>
       </c>
       <c r="E28" s="2" t="n">
         <v>0.7</v>
@@ -987,52 +987,52 @@
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>Call of Duty®: Black Ops III</t>
+          <t>Keep Talking and Nobody Explodes</t>
         </is>
       </c>
       <c r="B29" s="2" t="n">
-        <v>0.86</v>
+        <v>0.97</v>
       </c>
       <c r="C29" s="3" t="n">
-        <v>116101</v>
+        <v>10784</v>
       </c>
       <c r="D29" s="4" t="n">
-        <v>19.79</v>
+        <v>4.43</v>
       </c>
       <c r="E29" s="2" t="n">
-        <v>0.67</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>Deep Rock Galactic</t>
+          <t>Human Fall Flat</t>
         </is>
       </c>
       <c r="B30" s="2" t="n">
-        <v>0.97</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="C30" s="3" t="n">
-        <v>213323</v>
+        <v>149823</v>
       </c>
       <c r="D30" s="4" t="n">
-        <v>9.890000000000001</v>
+        <v>5.99</v>
       </c>
       <c r="E30" s="2" t="n">
-        <v>0.67</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>Call of Duty®: Black Ops Cold War</t>
+          <t>Call of Duty®: Black Ops III</t>
         </is>
       </c>
       <c r="B31" s="2" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.86</v>
       </c>
       <c r="C31" s="3" t="n">
-        <v>10560</v>
+        <v>116103</v>
       </c>
       <c r="D31" s="4" t="n">
         <v>19.79</v>
@@ -1044,17 +1044,17 @@
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>Call of Duty®: Black Ops II</t>
+          <t>Deep Rock Galactic</t>
         </is>
       </c>
       <c r="B32" s="2" t="n">
-        <v>0.86</v>
+        <v>0.97</v>
       </c>
       <c r="C32" s="3" t="n">
-        <v>18232</v>
+        <v>213340</v>
       </c>
       <c r="D32" s="4" t="n">
-        <v>19.79</v>
+        <v>9.890000000000001</v>
       </c>
       <c r="E32" s="2" t="n">
         <v>0.67</v>
@@ -1063,17 +1063,17 @@
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>Ori and the Will of the Wisps</t>
+          <t>Call of Duty®: Black Ops Cold War</t>
         </is>
       </c>
       <c r="B33" s="2" t="n">
-        <v>0.96</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="C33" s="3" t="n">
-        <v>112324</v>
+        <v>10560</v>
       </c>
       <c r="D33" s="4" t="n">
-        <v>9.890000000000001</v>
+        <v>19.79</v>
       </c>
       <c r="E33" s="2" t="n">
         <v>0.67</v>
@@ -1082,17 +1082,17 @@
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>Little Nightmares II</t>
+          <t>Call of Duty®: Black Ops II</t>
         </is>
       </c>
       <c r="B34" s="2" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.86</v>
       </c>
       <c r="C34" s="3" t="n">
-        <v>26807</v>
+        <v>18232</v>
       </c>
       <c r="D34" s="4" t="n">
-        <v>9.890000000000001</v>
+        <v>19.79</v>
       </c>
       <c r="E34" s="2" t="n">
         <v>0.67</v>
@@ -1101,14 +1101,14 @@
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>Insurgency: Sandstorm</t>
+          <t>Little Nightmares II</t>
         </is>
       </c>
       <c r="B35" s="2" t="n">
-        <v>0.86</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="C35" s="3" t="n">
-        <v>89328</v>
+        <v>26808</v>
       </c>
       <c r="D35" s="4" t="n">
         <v>9.890000000000001</v>
@@ -1120,74 +1120,74 @@
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>Hunt: Showdown</t>
+          <t>Insurgency: Sandstorm</t>
         </is>
       </c>
       <c r="B36" s="2" t="n">
-        <v>0.83</v>
+        <v>0.86</v>
       </c>
       <c r="C36" s="3" t="n">
-        <v>148433</v>
+        <v>89331</v>
       </c>
       <c r="D36" s="4" t="n">
-        <v>13.99</v>
+        <v>9.890000000000001</v>
       </c>
       <c r="E36" s="2" t="n">
-        <v>0.65</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>We Were Here Together</t>
+          <t>Hunt: Showdown</t>
         </is>
       </c>
       <c r="B37" s="2" t="n">
-        <v>0.85</v>
+        <v>0.83</v>
       </c>
       <c r="C37" s="3" t="n">
-        <v>10212</v>
+        <v>148438</v>
       </c>
       <c r="D37" s="4" t="n">
-        <v>4.93</v>
+        <v>13.99</v>
       </c>
       <c r="E37" s="2" t="n">
-        <v>0.62</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>Tom Clancy's Rainbow Six® Siege</t>
+          <t>We Were Here Together</t>
         </is>
       </c>
       <c r="B38" s="2" t="n">
-        <v>0.86</v>
+        <v>0.85</v>
       </c>
       <c r="C38" s="3" t="n">
-        <v>1025211</v>
+        <v>10215</v>
       </c>
       <c r="D38" s="4" t="n">
-        <v>7.99</v>
+        <v>4.93</v>
       </c>
       <c r="E38" s="2" t="n">
-        <v>0.6</v>
+        <v>0.62</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>Rain World</t>
+          <t>Tom Clancy's Rainbow Six® Siege</t>
         </is>
       </c>
       <c r="B39" s="2" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.86</v>
       </c>
       <c r="C39" s="3" t="n">
-        <v>19792</v>
+        <v>1025238</v>
       </c>
       <c r="D39" s="4" t="n">
-        <v>9.800000000000001</v>
+        <v>7.99</v>
       </c>
       <c r="E39" s="2" t="n">
         <v>0.6</v>
@@ -1196,17 +1196,17 @@
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>Metal: Hellsinger</t>
+          <t>Rain World</t>
         </is>
       </c>
       <c r="B40" s="2" t="n">
-        <v>0.96</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="C40" s="3" t="n">
-        <v>10738</v>
+        <v>19794</v>
       </c>
       <c r="D40" s="4" t="n">
-        <v>11.99</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="E40" s="2" t="n">
         <v>0.6</v>
@@ -1234,39 +1234,39 @@
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>Ultimate Chicken Horse</t>
+          <t>High On Life</t>
         </is>
       </c>
       <c r="B42" s="2" t="n">
-        <v>0.96</v>
+        <v>0.89</v>
       </c>
       <c r="C42" s="3" t="n">
-        <v>29447</v>
+        <v>13172</v>
       </c>
       <c r="D42" s="4" t="n">
-        <v>5.84</v>
+        <v>24.53</v>
       </c>
       <c r="E42" s="2" t="n">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>High On Life</t>
+          <t>Atomic Heart</t>
         </is>
       </c>
       <c r="B43" s="2" t="n">
-        <v>0.89</v>
+        <v>0.84</v>
       </c>
       <c r="C43" s="3" t="n">
-        <v>13171</v>
+        <v>21445</v>
       </c>
       <c r="D43" s="4" t="n">
-        <v>24.53</v>
+        <v>29.99</v>
       </c>
       <c r="E43" s="2" t="n">
-        <v>0.54</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="44">
@@ -1279,7 +1279,7 @@
         <v>0.84</v>
       </c>
       <c r="C44" s="3" t="n">
-        <v>21442</v>
+        <v>21445</v>
       </c>
       <c r="D44" s="4" t="n">
         <v>29.99</v>
@@ -1298,7 +1298,7 @@
         <v>0.83</v>
       </c>
       <c r="C45" s="3" t="n">
-        <v>119705</v>
+        <v>119714</v>
       </c>
       <c r="D45" s="4" t="n">
         <v>22.49</v>
@@ -1317,7 +1317,7 @@
         <v>0.97</v>
       </c>
       <c r="C46" s="3" t="n">
-        <v>290251</v>
+        <v>290262</v>
       </c>
       <c r="D46" s="4" t="n">
         <v>7.39</v>
@@ -1336,7 +1336,7 @@
         <v>0.92</v>
       </c>
       <c r="C47" s="3" t="n">
-        <v>23436</v>
+        <v>23438</v>
       </c>
       <c r="D47" s="4" t="n">
         <v>9.99</v>
@@ -1355,7 +1355,7 @@
         <v>0.91</v>
       </c>
       <c r="C48" s="3" t="n">
-        <v>16890</v>
+        <v>16889</v>
       </c>
       <c r="D48" s="4" t="n">
         <v>19.99</v>
@@ -1367,17 +1367,17 @@
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>MechWarrior 5: Mercenaries</t>
+          <t>Sackboy™: A Big Adventure</t>
         </is>
       </c>
       <c r="B49" s="2" t="n">
-        <v>0.84</v>
+        <v>0.85</v>
       </c>
       <c r="C49" s="3" t="n">
-        <v>8242</v>
+        <v>1327</v>
       </c>
       <c r="D49" s="4" t="n">
-        <v>14.99</v>
+        <v>29.99</v>
       </c>
       <c r="E49" s="2" t="n">
         <v>0.5</v>
@@ -1386,17 +1386,17 @@
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>Sackboy™: A Big Adventure</t>
+          <t>Call of Duty®: Modern Warfare® 3 (2011)</t>
         </is>
       </c>
       <c r="B50" s="2" t="n">
-        <v>0.85</v>
+        <v>0.89</v>
       </c>
       <c r="C50" s="3" t="n">
-        <v>1327</v>
+        <v>12366</v>
       </c>
       <c r="D50" s="4" t="n">
-        <v>29.99</v>
+        <v>19.99</v>
       </c>
       <c r="E50" s="2" t="n">
         <v>0.5</v>
@@ -1405,14 +1405,14 @@
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>Call of Duty®: Modern Warfare® 3 (2011)</t>
+          <t>Shovel Knight: Treasure Trove</t>
         </is>
       </c>
       <c r="B51" s="2" t="n">
-        <v>0.89</v>
+        <v>0.95</v>
       </c>
       <c r="C51" s="3" t="n">
-        <v>12366</v>
+        <v>12826</v>
       </c>
       <c r="D51" s="4" t="n">
         <v>19.99</v>
@@ -1431,7 +1431,7 @@
         <v>0.95</v>
       </c>
       <c r="C52" s="3" t="n">
-        <v>8523</v>
+        <v>8525</v>
       </c>
       <c r="D52" s="4" t="n">
         <v>7.39</v>
@@ -1443,55 +1443,55 @@
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
         <is>
-          <t>Shovel Knight: Treasure Trove</t>
+          <t>We Were Here Forever</t>
         </is>
       </c>
       <c r="B53" s="2" t="n">
-        <v>0.95</v>
+        <v>0.91</v>
       </c>
       <c r="C53" s="3" t="n">
-        <v>12823</v>
+        <v>10360</v>
       </c>
       <c r="D53" s="4" t="n">
-        <v>19.99</v>
+        <v>9.890000000000001</v>
       </c>
       <c r="E53" s="2" t="n">
-        <v>0.5</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
         <is>
-          <t>We Were Here Forever</t>
+          <t>BattleBit Remastered</t>
         </is>
       </c>
       <c r="B54" s="2" t="n">
-        <v>0.91</v>
+        <v>0.9</v>
       </c>
       <c r="C54" s="3" t="n">
-        <v>10360</v>
+        <v>104945</v>
       </c>
       <c r="D54" s="4" t="n">
-        <v>9.890000000000001</v>
+        <v>8.869999999999999</v>
       </c>
       <c r="E54" s="2" t="n">
-        <v>0.45</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
         <is>
-          <t>BattleBit Remastered</t>
+          <t>GTFO</t>
         </is>
       </c>
       <c r="B55" s="2" t="n">
-        <v>0.9</v>
+        <v>0.87</v>
       </c>
       <c r="C55" s="3" t="n">
-        <v>104930</v>
+        <v>37182</v>
       </c>
       <c r="D55" s="4" t="n">
-        <v>8.869999999999999</v>
+        <v>23.99</v>
       </c>
       <c r="E55" s="2" t="n">
         <v>0.4</v>
@@ -1507,7 +1507,7 @@
         <v>0.87</v>
       </c>
       <c r="C56" s="3" t="n">
-        <v>37181</v>
+        <v>37182</v>
       </c>
       <c r="D56" s="4" t="n">
         <v>23.99</v>
@@ -1526,7 +1526,7 @@
         <v>0.96</v>
       </c>
       <c r="C57" s="3" t="n">
-        <v>22867</v>
+        <v>22871</v>
       </c>
       <c r="D57" s="4" t="n">
         <v>7.79</v>
@@ -1545,7 +1545,7 @@
         <v>0.84</v>
       </c>
       <c r="C58" s="3" t="n">
-        <v>72361</v>
+        <v>72362</v>
       </c>
       <c r="D58" s="4" t="n">
         <v>29.24</v>
@@ -1564,7 +1564,7 @@
         <v>0.9</v>
       </c>
       <c r="C59" s="3" t="n">
-        <v>5907</v>
+        <v>5908</v>
       </c>
       <c r="D59" s="4" t="n">
         <v>9.74</v>
@@ -1621,7 +1621,7 @@
         <v>0.9399999999999999</v>
       </c>
       <c r="C62" s="3" t="n">
-        <v>5173</v>
+        <v>5174</v>
       </c>
       <c r="D62" s="4" t="n">
         <v>20.09</v>
@@ -1640,7 +1640,7 @@
         <v>0.96</v>
       </c>
       <c r="C63" s="3" t="n">
-        <v>21610</v>
+        <v>21614</v>
       </c>
       <c r="D63" s="4" t="n">
         <v>13.06</v>
@@ -1678,7 +1678,7 @@
         <v>0.96</v>
       </c>
       <c r="C65" s="3" t="n">
-        <v>134777</v>
+        <v>134784</v>
       </c>
       <c r="D65" s="4" t="n">
         <v>13.99</v>
@@ -1697,7 +1697,7 @@
         <v>0.92</v>
       </c>
       <c r="C66" s="3" t="n">
-        <v>9663</v>
+        <v>9664</v>
       </c>
       <c r="D66" s="4" t="n">
         <v>20.29</v>
@@ -1728,17 +1728,17 @@
     <row r="68">
       <c r="A68" s="1" t="inlineStr">
         <is>
-          <t>The Case of the Golden Idol</t>
+          <t>Terra Nil</t>
         </is>
       </c>
       <c r="B68" s="2" t="n">
-        <v>0.98</v>
+        <v>0.85</v>
       </c>
       <c r="C68" s="3" t="n">
-        <v>4768</v>
+        <v>4392</v>
       </c>
       <c r="D68" s="4" t="n">
-        <v>12.59</v>
+        <v>17.49</v>
       </c>
       <c r="E68" s="2" t="n">
         <v>0.3</v>
@@ -1747,17 +1747,17 @@
     <row r="69">
       <c r="A69" s="1" t="inlineStr">
         <is>
-          <t>Baba Is You</t>
+          <t>The Case of the Golden Idol</t>
         </is>
       </c>
       <c r="B69" s="2" t="n">
         <v>0.98</v>
       </c>
       <c r="C69" s="3" t="n">
-        <v>16244</v>
+        <v>4768</v>
       </c>
       <c r="D69" s="4" t="n">
-        <v>8.74</v>
+        <v>12.59</v>
       </c>
       <c r="E69" s="2" t="n">
         <v>0.3</v>
@@ -1773,7 +1773,7 @@
         <v>0.95</v>
       </c>
       <c r="C70" s="3" t="n">
-        <v>2125</v>
+        <v>2126</v>
       </c>
       <c r="D70" s="4" t="n">
         <v>11.75</v>
@@ -1785,36 +1785,36 @@
     <row r="71">
       <c r="A71" s="1" t="inlineStr">
         <is>
-          <t>Six Days in Fallujah</t>
+          <t>Baba Is You</t>
         </is>
       </c>
       <c r="B71" s="2" t="n">
-        <v>0.86</v>
+        <v>0.98</v>
       </c>
       <c r="C71" s="3" t="n">
-        <v>7533</v>
+        <v>16246</v>
       </c>
       <c r="D71" s="4" t="n">
-        <v>29.24</v>
+        <v>8.74</v>
       </c>
       <c r="E71" s="2" t="n">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="inlineStr">
         <is>
-          <t>ULTRAKILL</t>
+          <t>Six Days in Fallujah</t>
         </is>
       </c>
       <c r="B72" s="2" t="n">
-        <v>0.98</v>
+        <v>0.86</v>
       </c>
       <c r="C72" s="3" t="n">
-        <v>81134</v>
+        <v>7533</v>
       </c>
       <c r="D72" s="4" t="n">
-        <v>15.74</v>
+        <v>29.24</v>
       </c>
       <c r="E72" s="2" t="n">
         <v>0.25</v>
@@ -1823,17 +1823,17 @@
     <row r="73">
       <c r="A73" s="1" t="inlineStr">
         <is>
-          <t>Roboquest</t>
+          <t>ULTRAKILL</t>
         </is>
       </c>
       <c r="B73" s="2" t="n">
-        <v>0.95</v>
+        <v>0.98</v>
       </c>
       <c r="C73" s="3" t="n">
-        <v>8716</v>
+        <v>81149</v>
       </c>
       <c r="D73" s="4" t="n">
-        <v>18.74</v>
+        <v>15.74</v>
       </c>
       <c r="E73" s="2" t="n">
         <v>0.25</v>
@@ -1842,17 +1842,17 @@
     <row r="74">
       <c r="A74" s="1" t="inlineStr">
         <is>
-          <t>Escape Simulator</t>
+          <t>Roboquest</t>
         </is>
       </c>
       <c r="B74" s="2" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.95</v>
       </c>
       <c r="C74" s="3" t="n">
-        <v>11388</v>
+        <v>8719</v>
       </c>
       <c r="D74" s="4" t="n">
-        <v>11.24</v>
+        <v>18.74</v>
       </c>
       <c r="E74" s="2" t="n">
         <v>0.25</v>
@@ -1861,17 +1861,17 @@
     <row r="75">
       <c r="A75" s="1" t="inlineStr">
         <is>
-          <t>Gunfire Reborn</t>
+          <t>Escape Simulator</t>
         </is>
       </c>
       <c r="B75" s="2" t="n">
-        <v>0.93</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="C75" s="3" t="n">
-        <v>78856</v>
+        <v>11388</v>
       </c>
       <c r="D75" s="4" t="n">
-        <v>12.59</v>
+        <v>11.24</v>
       </c>
       <c r="E75" s="2" t="n">
         <v>0.25</v>
@@ -1880,17 +1880,17 @@
     <row r="76">
       <c r="A76" s="1" t="inlineStr">
         <is>
-          <t>Pizza Tower</t>
+          <t>Gunfire Reborn</t>
         </is>
       </c>
       <c r="B76" s="2" t="n">
-        <v>0.98</v>
+        <v>0.93</v>
       </c>
       <c r="C76" s="3" t="n">
-        <v>45210</v>
+        <v>78858</v>
       </c>
       <c r="D76" s="4" t="n">
-        <v>14.62</v>
+        <v>12.59</v>
       </c>
       <c r="E76" s="2" t="n">
         <v>0.25</v>
@@ -1899,17 +1899,17 @@
     <row r="77">
       <c r="A77" s="1" t="inlineStr">
         <is>
-          <t>Viewfinder</t>
+          <t>Pizza Tower</t>
         </is>
       </c>
       <c r="B77" s="2" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.98</v>
       </c>
       <c r="C77" s="3" t="n">
-        <v>4389</v>
+        <v>45214</v>
       </c>
       <c r="D77" s="4" t="n">
-        <v>18.74</v>
+        <v>14.62</v>
       </c>
       <c r="E77" s="2" t="n">
         <v>0.25</v>
@@ -1918,74 +1918,74 @@
     <row r="78">
       <c r="A78" s="1" t="inlineStr">
         <is>
-          <t>The Talos Principle 2</t>
+          <t>Viewfinder</t>
         </is>
       </c>
       <c r="B78" s="2" t="n">
-        <v>0.96</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="C78" s="3" t="n">
-        <v>6066</v>
+        <v>4389</v>
       </c>
       <c r="D78" s="4" t="n">
-        <v>23.19</v>
+        <v>18.74</v>
       </c>
       <c r="E78" s="2" t="n">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="inlineStr">
         <is>
-          <t>Chants of Sennaar</t>
+          <t>Squad 44</t>
         </is>
       </c>
       <c r="B79" s="2" t="n">
-        <v>0.98</v>
+        <v>0.8</v>
       </c>
       <c r="C79" s="3" t="n">
-        <v>7772</v>
+        <v>15817</v>
       </c>
       <c r="D79" s="4" t="n">
-        <v>15.99</v>
+        <v>21</v>
       </c>
       <c r="E79" s="2" t="n">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="inlineStr">
         <is>
-          <t>Jusant</t>
+          <t>Sticky Business</t>
         </is>
       </c>
       <c r="B80" s="2" t="n">
-        <v>0.96</v>
+        <v>0.97</v>
       </c>
       <c r="C80" s="3" t="n">
-        <v>1160</v>
+        <v>2805</v>
       </c>
       <c r="D80" s="4" t="n">
-        <v>19.99</v>
+        <v>7.49</v>
       </c>
       <c r="E80" s="2" t="n">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="inlineStr">
         <is>
-          <t>COCOON</t>
+          <t>The Talos Principle 2</t>
         </is>
       </c>
       <c r="B81" s="2" t="n">
         <v>0.96</v>
       </c>
       <c r="C81" s="3" t="n">
-        <v>2883</v>
+        <v>6070</v>
       </c>
       <c r="D81" s="4" t="n">
-        <v>18.39</v>
+        <v>23.19</v>
       </c>
       <c r="E81" s="2" t="n">
         <v>0.2</v>
@@ -1994,74 +1994,74 @@
     <row r="82">
       <c r="A82" s="1" t="inlineStr">
         <is>
-          <t>Mini Motorways</t>
+          <t>Chants of Sennaar</t>
         </is>
       </c>
       <c r="B82" s="2" t="n">
-        <v>0.95</v>
+        <v>0.98</v>
       </c>
       <c r="C82" s="3" t="n">
-        <v>17414</v>
+        <v>7775</v>
       </c>
       <c r="D82" s="4" t="n">
-        <v>7.37</v>
+        <v>15.99</v>
       </c>
       <c r="E82" s="2" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="inlineStr">
         <is>
-          <t>Team Fortress 2</t>
+          <t>Jusant</t>
         </is>
       </c>
       <c r="B83" s="2" t="n">
-        <v>0.93</v>
+        <v>0.96</v>
       </c>
       <c r="C83" s="3" t="n">
-        <v>1018966</v>
+        <v>1160</v>
       </c>
       <c r="D83" s="4" t="n">
-        <v>0</v>
+        <v>19.99</v>
       </c>
       <c r="E83" s="2" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="inlineStr">
         <is>
-          <t>Fireworks Mania - An Explosive Simulator</t>
+          <t>COCOON</t>
         </is>
       </c>
       <c r="B84" s="2" t="n">
         <v>0.96</v>
       </c>
       <c r="C84" s="3" t="n">
-        <v>4674</v>
+        <v>2884</v>
       </c>
       <c r="D84" s="4" t="n">
-        <v>9.99</v>
+        <v>18.39</v>
       </c>
       <c r="E84" s="2" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="inlineStr">
         <is>
-          <t>GROUND BRANCH</t>
+          <t>Team Fortress 2</t>
         </is>
       </c>
       <c r="B85" s="2" t="n">
-        <v>0.91</v>
+        <v>0.93</v>
       </c>
       <c r="C85" s="3" t="n">
-        <v>14919</v>
+        <v>1018978</v>
       </c>
       <c r="D85" s="4" t="n">
-        <v>24.99</v>
+        <v>0</v>
       </c>
       <c r="E85" s="2" t="n">
         <v>0</v>
@@ -2070,19 +2070,57 @@
     <row r="86">
       <c r="A86" s="1" t="inlineStr">
         <is>
+          <t>Fireworks Mania - An Explosive Simulator</t>
+        </is>
+      </c>
+      <c r="B86" s="2" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="C86" s="3" t="n">
+        <v>4675</v>
+      </c>
+      <c r="D86" s="4" t="n">
+        <v>9.99</v>
+      </c>
+      <c r="E86" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="inlineStr">
+        <is>
+          <t>GROUND BRANCH</t>
+        </is>
+      </c>
+      <c r="B87" s="2" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="C87" s="3" t="n">
+        <v>14919</v>
+      </c>
+      <c r="D87" s="4" t="n">
+        <v>24.99</v>
+      </c>
+      <c r="E87" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="inlineStr">
+        <is>
           <t>Ori and the Blind Forest</t>
         </is>
       </c>
-      <c r="B86" s="2" t="n">
+      <c r="B88" s="2" t="n">
         <v>0.95</v>
       </c>
-      <c r="C86" s="3" t="n">
-        <v>44812</v>
-      </c>
-      <c r="D86" s="4" t="n">
+      <c r="C88" s="3" t="n">
+        <v>44811</v>
+      </c>
+      <c r="D88" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="E86" s="2" t="n">
+      <c r="E88" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2173,6 +2211,8 @@
     <hyperlink ref="A84" r:id="rId83"/>
     <hyperlink ref="A85" r:id="rId84"/>
     <hyperlink ref="A86" r:id="rId85"/>
+    <hyperlink ref="A87" r:id="rId86"/>
+    <hyperlink ref="A88" r:id="rId87"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
made input settings not constant
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -480,340 +480,340 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>Airport CEO</t>
+          <t>Borderlands 3</t>
         </is>
       </c>
       <c r="B2" s="4" t="n">
-        <v>0.84</v>
+        <v>0.85</v>
       </c>
       <c r="C2" s="5" t="n">
-        <v>6438</v>
+        <v>99074</v>
       </c>
       <c r="D2" s="6" t="n">
-        <v>6.12</v>
+        <v>8.99</v>
       </c>
       <c r="E2" s="4" t="n">
-        <v>0.75</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>F1® Manager 2023</t>
+          <t>BioShock Infinite</t>
         </is>
       </c>
       <c r="B3" s="4" t="n">
-        <v>0.76</v>
+        <v>0.93</v>
       </c>
       <c r="C3" s="5" t="n">
-        <v>1326</v>
+        <v>100694</v>
       </c>
       <c r="D3" s="6" t="n">
-        <v>16.49</v>
+        <v>7.49</v>
       </c>
       <c r="E3" s="4" t="n">
-        <v>0.7</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>Electrician Simulator</t>
+          <t>Hell Let Loose</t>
         </is>
       </c>
       <c r="B4" s="4" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.84</v>
       </c>
       <c r="C4" s="5" t="n">
-        <v>1450</v>
+        <v>73081</v>
       </c>
       <c r="D4" s="6" t="n">
-        <v>7.19</v>
+        <v>29.24</v>
       </c>
       <c r="E4" s="4" t="n">
-        <v>0.6</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>Lawn Mowing Simulator</t>
+          <t>Trepang2</t>
         </is>
       </c>
       <c r="B5" s="4" t="n">
-        <v>0.76</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="C5" s="5" t="n">
-        <v>1581</v>
+        <v>5445</v>
       </c>
       <c r="D5" s="6" t="n">
-        <v>11.99</v>
+        <v>20.09</v>
       </c>
       <c r="E5" s="4" t="n">
-        <v>0.6</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>Pets Hotel</t>
+          <t>Warhammer 40,000: Boltgun</t>
         </is>
       </c>
       <c r="B6" s="4" t="n">
-        <v>0.85</v>
+        <v>0.91</v>
       </c>
       <c r="C6" s="5" t="n">
-        <v>135</v>
+        <v>9774</v>
       </c>
       <c r="D6" s="6" t="n">
-        <v>8.390000000000001</v>
+        <v>14.95</v>
       </c>
       <c r="E6" s="4" t="n">
-        <v>0.52</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>Farmer's Life</t>
+          <t>COCOON</t>
         </is>
       </c>
       <c r="B7" s="4" t="n">
-        <v>0.86</v>
+        <v>0.95</v>
       </c>
       <c r="C7" s="5" t="n">
-        <v>1417</v>
+        <v>3262</v>
       </c>
       <c r="D7" s="6" t="n">
-        <v>16.39</v>
+        <v>16.09</v>
       </c>
       <c r="E7" s="4" t="n">
-        <v>0.44</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>Hotel Renovator</t>
+          <t>Roboquest</t>
         </is>
       </c>
       <c r="B8" s="4" t="n">
-        <v>0.78</v>
+        <v>0.95</v>
       </c>
       <c r="C8" s="5" t="n">
-        <v>1529</v>
+        <v>9633</v>
       </c>
       <c r="D8" s="6" t="n">
-        <v>14.99</v>
+        <v>18.74</v>
       </c>
       <c r="E8" s="4" t="n">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>Trade Bots: A Technical Analysis Simulation</t>
+          <t>Fireworks Mania - An Explosive Simulator</t>
         </is>
       </c>
       <c r="B9" s="4" t="n">
-        <v>0.83</v>
+        <v>0.96</v>
       </c>
       <c r="C9" s="5" t="n">
-        <v>31</v>
+        <v>4813</v>
       </c>
       <c r="D9" s="6" t="n">
-        <v>7.07</v>
+        <v>7.99</v>
       </c>
       <c r="E9" s="4" t="n">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>Alaskan Road Truckers</t>
+          <t>Tom Clancy's Rainbow Six® Siege</t>
         </is>
       </c>
       <c r="B10" s="4" t="n">
-        <v>0.66</v>
+        <v>0.86</v>
       </c>
       <c r="C10" s="5" t="n">
-        <v>1996</v>
+        <v>1032092</v>
       </c>
       <c r="D10" s="6" t="n">
-        <v>21.14</v>
+        <v>19.99</v>
       </c>
       <c r="E10" s="4" t="n">
-        <v>0.33</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>Music Store Simulator</t>
+          <t>Team Fortress 2</t>
         </is>
       </c>
       <c r="B11" s="4" t="n">
-        <v>0.82</v>
+        <v>0.93</v>
       </c>
       <c r="C11" s="5" t="n">
-        <v>97</v>
+        <v>1022451</v>
       </c>
       <c r="D11" s="6" t="n">
-        <v>23.84</v>
+        <v>0</v>
       </c>
       <c r="E11" s="4" t="n">
-        <v>0.31</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>Storage Hustle</t>
+          <t>BattleBit Remastered</t>
         </is>
       </c>
       <c r="B12" s="4" t="n">
-        <v>0.83</v>
+        <v>0.9</v>
       </c>
       <c r="C12" s="5" t="n">
-        <v>379</v>
+        <v>107017</v>
       </c>
       <c r="D12" s="6" t="n">
-        <v>8.25</v>
+        <v>14.79</v>
       </c>
       <c r="E12" s="4" t="n">
-        <v>0.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>Travellers Rest</t>
+          <t>Deep Rock Galactic</t>
         </is>
       </c>
       <c r="B13" s="4" t="n">
-        <v>0.9</v>
+        <v>0.97</v>
       </c>
       <c r="C13" s="5" t="n">
-        <v>7383</v>
+        <v>215574</v>
       </c>
       <c r="D13" s="6" t="n">
-        <v>11.09</v>
+        <v>29.99</v>
       </c>
       <c r="E13" s="4" t="n">
-        <v>0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>Software Inc.</t>
+          <t>ULTRAKILL</t>
         </is>
       </c>
       <c r="B14" s="4" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.98</v>
       </c>
       <c r="C14" s="5" t="n">
-        <v>6187</v>
+        <v>83731</v>
       </c>
       <c r="D14" s="6" t="n">
-        <v>16.9</v>
+        <v>24.5</v>
       </c>
       <c r="E14" s="4" t="n">
-        <v>0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>ACRES</t>
+          <t>Inscryption</t>
         </is>
       </c>
       <c r="B15" s="4" t="n">
-        <v>0.84</v>
+        <v>0.96</v>
       </c>
       <c r="C15" s="5" t="n">
-        <v>111</v>
+        <v>96881</v>
       </c>
       <c r="D15" s="6" t="n">
-        <v>11.83</v>
+        <v>19.99</v>
       </c>
       <c r="E15" s="4" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>My Supermarket</t>
+          <t>Gunfire Reborn</t>
         </is>
       </c>
       <c r="B16" s="4" t="n">
-        <v>0.96</v>
+        <v>0.93</v>
       </c>
       <c r="C16" s="5" t="n">
-        <v>91</v>
+        <v>79152</v>
       </c>
       <c r="D16" s="6" t="n">
-        <v>11.83</v>
+        <v>16.79</v>
       </c>
       <c r="E16" s="4" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>Tribe: Primitive Builder</t>
+          <t>A Little to the Left</t>
         </is>
       </c>
       <c r="B17" s="4" t="n">
-        <v>0.83</v>
+        <v>0.91</v>
       </c>
       <c r="C17" s="5" t="n">
-        <v>408</v>
+        <v>6209</v>
       </c>
       <c r="D17" s="6" t="n">
-        <v>18.52</v>
+        <v>14.99</v>
       </c>
       <c r="E17" s="4" t="n">
-        <v>0.19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>Computer Repair Shop</t>
+          <t>Metal: Hellsinger</t>
         </is>
       </c>
       <c r="B18" s="4" t="n">
-        <v>0.63</v>
+        <v>0.96</v>
       </c>
       <c r="C18" s="5" t="n">
-        <v>63</v>
+        <v>10895</v>
       </c>
       <c r="D18" s="6" t="n">
-        <v>8.279999999999999</v>
+        <v>29.99</v>
       </c>
       <c r="E18" s="4" t="n">
-        <v>0.15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>Mind Over Magic</t>
+          <t>Left 4 Dead 2</t>
         </is>
       </c>
       <c r="B19" s="4" t="n">
-        <v>0.91</v>
+        <v>0.97</v>
       </c>
       <c r="C19" s="5" t="n">
-        <v>887</v>
+        <v>614416</v>
       </c>
       <c r="D19" s="6" t="n">
-        <v>22.99</v>
+        <v>9.75</v>
       </c>
       <c r="E19" s="4" t="n">
         <v>0</v>
@@ -822,17 +822,17 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>Police Simulator: Patrol Officers</t>
+          <t>The Talos Principle 2</t>
         </is>
       </c>
       <c r="B20" s="4" t="n">
-        <v>0.83</v>
+        <v>0.95</v>
       </c>
       <c r="C20" s="5" t="n">
-        <v>11899</v>
+        <v>6562</v>
       </c>
       <c r="D20" s="6" t="n">
-        <v>29.99</v>
+        <v>28.99</v>
       </c>
       <c r="E20" s="4" t="n">
         <v>0</v>
@@ -841,17 +841,17 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>Shadows of Doubt</t>
+          <t>Escape Simulator</t>
         </is>
       </c>
       <c r="B21" s="4" t="n">
-        <v>0.92</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="C21" s="5" t="n">
-        <v>7338</v>
+        <v>11499</v>
       </c>
       <c r="D21" s="6" t="n">
-        <v>19.99</v>
+        <v>14.99</v>
       </c>
       <c r="E21" s="4" t="n">
         <v>0</v>
@@ -860,17 +860,17 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>Stormworks: Build and Rescue</t>
+          <t>Portal 2</t>
         </is>
       </c>
       <c r="B22" s="4" t="n">
-        <v>0.89</v>
+        <v>0.98</v>
       </c>
       <c r="C22" s="5" t="n">
-        <v>39739</v>
+        <v>310744</v>
       </c>
       <c r="D22" s="6" t="n">
-        <v>24.5</v>
+        <v>9.75</v>
       </c>
       <c r="E22" s="4" t="n">
         <v>0</v>
@@ -879,17 +879,17 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>Eco</t>
+          <t>We Were Here Forever</t>
         </is>
       </c>
       <c r="B23" s="4" t="n">
-        <v>0.82</v>
+        <v>0.91</v>
       </c>
       <c r="C23" s="5" t="n">
-        <v>9523</v>
+        <v>10575</v>
       </c>
       <c r="D23" s="6" t="n">
-        <v>28.99</v>
+        <v>17.99</v>
       </c>
       <c r="E23" s="4" t="n">
         <v>0</v>
@@ -898,17 +898,17 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>The Exit 8</t>
+          <t>Chants of Sennaar</t>
         </is>
       </c>
       <c r="B24" s="4" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.98</v>
       </c>
       <c r="C24" s="5" t="n">
-        <v>3939</v>
+        <v>8513</v>
       </c>
       <c r="D24" s="6" t="n">
-        <v>3.99</v>
+        <v>19.99</v>
       </c>
       <c r="E24" s="4" t="n">
         <v>0</v>
@@ -917,17 +917,17 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>Barony</t>
+          <t>GROUND BRANCH</t>
         </is>
       </c>
       <c r="B25" s="4" t="n">
-        <v>0.92</v>
+        <v>0.91</v>
       </c>
       <c r="C25" s="5" t="n">
-        <v>4493</v>
+        <v>15076</v>
       </c>
       <c r="D25" s="6" t="n">
-        <v>19.5</v>
+        <v>24.99</v>
       </c>
       <c r="E25" s="4" t="n">
         <v>0</v>
@@ -936,17 +936,17 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>Flyout</t>
+          <t>PAYDAY 2</t>
         </is>
       </c>
       <c r="B26" s="4" t="n">
         <v>0.89</v>
       </c>
       <c r="C26" s="5" t="n">
-        <v>710</v>
+        <v>423660</v>
       </c>
       <c r="D26" s="6" t="n">
-        <v>19.99</v>
+        <v>9.99</v>
       </c>
       <c r="E26" s="4" t="n">
         <v>0</v>
@@ -955,17 +955,17 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>Cruelty Squad</t>
+          <t>Far Cry® 4</t>
         </is>
       </c>
       <c r="B27" s="4" t="n">
-        <v>0.97</v>
+        <v>0.83</v>
       </c>
       <c r="C27" s="5" t="n">
-        <v>14022</v>
+        <v>46590</v>
       </c>
       <c r="D27" s="6" t="n">
-        <v>16.79</v>
+        <v>29.99</v>
       </c>
       <c r="E27" s="4" t="n">
         <v>0</v>
@@ -974,17 +974,17 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>Car For Sale Simulator 2023</t>
+          <t>Jusant</t>
         </is>
       </c>
       <c r="B28" s="4" t="n">
-        <v>0.88</v>
+        <v>0.96</v>
       </c>
       <c r="C28" s="5" t="n">
-        <v>10679</v>
+        <v>1347</v>
       </c>
       <c r="D28" s="6" t="n">
-        <v>17.49</v>
+        <v>24.99</v>
       </c>
       <c r="E28" s="4" t="n">
         <v>0</v>
@@ -993,17 +993,17 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>Gym Simulator 24</t>
+          <t>SCP: 5K</t>
         </is>
       </c>
       <c r="B29" s="4" t="n">
-        <v>0.91</v>
+        <v>0.82</v>
       </c>
       <c r="C29" s="5" t="n">
-        <v>894</v>
+        <v>6685</v>
       </c>
       <c r="D29" s="6" t="n">
-        <v>10.79</v>
+        <v>19.5</v>
       </c>
       <c r="E29" s="4" t="n">
         <v>0</v>
@@ -1012,17 +1012,17 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>PC Building Simulator</t>
+          <t>Metro Exodus</t>
         </is>
       </c>
       <c r="B30" s="4" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.89</v>
       </c>
       <c r="C30" s="5" t="n">
-        <v>39405</v>
+        <v>86868</v>
       </c>
       <c r="D30" s="6" t="n">
-        <v>19.99</v>
+        <v>29.99</v>
       </c>
       <c r="E30" s="4" t="n">
         <v>0</v>
@@ -1031,17 +1031,17 @@
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>Tram Simulator Urban Transit</t>
+          <t>We Were Here Together</t>
         </is>
       </c>
       <c r="B31" s="4" t="n">
-        <v>0.57</v>
+        <v>0.85</v>
       </c>
       <c r="C31" s="5" t="n">
-        <v>109</v>
+        <v>10331</v>
       </c>
       <c r="D31" s="6" t="n">
-        <v>19.99</v>
+        <v>12.99</v>
       </c>
       <c r="E31" s="4" t="n">
         <v>0</v>
@@ -1050,17 +1050,17 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>Gunner, HEAT, PC!</t>
+          <t>MechWarrior 5: Mercenaries</t>
         </is>
       </c>
       <c r="B32" s="4" t="n">
-        <v>0.91</v>
+        <v>0.84</v>
       </c>
       <c r="C32" s="5" t="n">
-        <v>3131</v>
+        <v>8316</v>
       </c>
       <c r="D32" s="6" t="n">
-        <v>24.99</v>
+        <v>29.99</v>
       </c>
       <c r="E32" s="4" t="n">
         <v>0</v>
@@ -1069,14 +1069,14 @@
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>SimCity™ 4 Deluxe Edition</t>
+          <t>Call of Duty: World at War</t>
         </is>
       </c>
       <c r="B33" s="4" t="n">
-        <v>0.8</v>
+        <v>0.92</v>
       </c>
       <c r="C33" s="5" t="n">
-        <v>7073</v>
+        <v>39879</v>
       </c>
       <c r="D33" s="6" t="n">
         <v>19.99</v>
@@ -1088,17 +1088,17 @@
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>Placid Plastic Duck Simulator</t>
+          <t>Dorfromantik</t>
         </is>
       </c>
       <c r="B34" s="4" t="n">
-        <v>0.98</v>
+        <v>0.96</v>
       </c>
       <c r="C34" s="5" t="n">
-        <v>10472</v>
+        <v>23024</v>
       </c>
       <c r="D34" s="6" t="n">
-        <v>1.99</v>
+        <v>12.99</v>
       </c>
       <c r="E34" s="4" t="n">
         <v>0</v>
@@ -1107,17 +1107,17 @@
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>Gloomwood</t>
+          <t>Squad 44</t>
         </is>
       </c>
       <c r="B35" s="4" t="n">
-        <v>0.95</v>
+        <v>0.8</v>
       </c>
       <c r="C35" s="5" t="n">
-        <v>4213</v>
+        <v>15920</v>
       </c>
       <c r="D35" s="6" t="n">
-        <v>19.5</v>
+        <v>28</v>
       </c>
       <c r="E35" s="4" t="n">
         <v>0</v>
@@ -1126,17 +1126,17 @@
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>Mosa Lina</t>
+          <t>TUNIC</t>
         </is>
       </c>
       <c r="B36" s="4" t="n">
-        <v>0.96</v>
+        <v>0.92</v>
       </c>
       <c r="C36" s="5" t="n">
-        <v>751</v>
+        <v>9826</v>
       </c>
       <c r="D36" s="6" t="n">
-        <v>4.99</v>
+        <v>28.99</v>
       </c>
       <c r="E36" s="4" t="n">
         <v>0</v>
@@ -1145,266 +1145,19 @@
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>Chef Life: A Restaurant Simulator</t>
+          <t>Starship Troopers: Extermination</t>
         </is>
       </c>
       <c r="B37" s="4" t="n">
-        <v>0.83</v>
+        <v>0.89</v>
       </c>
       <c r="C37" s="5" t="n">
-        <v>927</v>
+        <v>23242</v>
       </c>
       <c r="D37" s="6" t="n">
-        <v>29.99</v>
+        <v>28.99</v>
       </c>
       <c r="E37" s="4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="3" t="inlineStr">
-        <is>
-          <t>NASCAR Heat 5</t>
-        </is>
-      </c>
-      <c r="B38" s="4" t="n">
-        <v>0.82</v>
-      </c>
-      <c r="C38" s="5" t="n">
-        <v>2241</v>
-      </c>
-      <c r="D38" s="6" t="n">
-        <v>14.79</v>
-      </c>
-      <c r="E38" s="4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="3" t="inlineStr">
-        <is>
-          <t>Void Bastards</t>
-        </is>
-      </c>
-      <c r="B39" s="4" t="n">
-        <v>0.87</v>
-      </c>
-      <c r="C39" s="5" t="n">
-        <v>3573</v>
-      </c>
-      <c r="D39" s="6" t="n">
-        <v>29.99</v>
-      </c>
-      <c r="E39" s="4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="3" t="inlineStr">
-        <is>
-          <t>Fish Game</t>
-        </is>
-      </c>
-      <c r="B40" s="4" t="n">
-        <v>0.93</v>
-      </c>
-      <c r="C40" s="5" t="n">
-        <v>233</v>
-      </c>
-      <c r="D40" s="6" t="n">
-        <v>24.5</v>
-      </c>
-      <c r="E40" s="4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="3" t="inlineStr">
-        <is>
-          <t>Ostranauts</t>
-        </is>
-      </c>
-      <c r="B41" s="4" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="C41" s="5" t="n">
-        <v>838</v>
-      </c>
-      <c r="D41" s="6" t="n">
-        <v>16.79</v>
-      </c>
-      <c r="E41" s="4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="3" t="inlineStr">
-        <is>
-          <t>KartKraft™</t>
-        </is>
-      </c>
-      <c r="B42" s="4" t="n">
-        <v>0.78</v>
-      </c>
-      <c r="C42" s="5" t="n">
-        <v>2330</v>
-      </c>
-      <c r="D42" s="6" t="n">
-        <v>24.5</v>
-      </c>
-      <c r="E42" s="4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="3" t="inlineStr">
-        <is>
-          <t>Rising Storm 2: Vietnam</t>
-        </is>
-      </c>
-      <c r="B43" s="4" t="n">
-        <v>0.87</v>
-      </c>
-      <c r="C43" s="5" t="n">
-        <v>37328</v>
-      </c>
-      <c r="D43" s="6" t="n">
-        <v>22.99</v>
-      </c>
-      <c r="E43" s="4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="3" t="inlineStr">
-        <is>
-          <t>Flight Of Nova</t>
-        </is>
-      </c>
-      <c r="B44" s="4" t="n">
-        <v>0.96</v>
-      </c>
-      <c r="C44" s="5" t="n">
-        <v>288</v>
-      </c>
-      <c r="D44" s="6" t="n">
-        <v>24.99</v>
-      </c>
-      <c r="E44" s="4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="3" t="inlineStr">
-        <is>
-          <t>Destroyer: The U-Boat Hunter</t>
-        </is>
-      </c>
-      <c r="B45" s="4" t="n">
-        <v>0.78</v>
-      </c>
-      <c r="C45" s="5" t="n">
-        <v>515</v>
-      </c>
-      <c r="D45" s="6" t="n">
-        <v>29.99</v>
-      </c>
-      <c r="E45" s="4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="3" t="inlineStr">
-        <is>
-          <t>The Magical Mixture Mill</t>
-        </is>
-      </c>
-      <c r="B46" s="4" t="n">
-        <v>0.83</v>
-      </c>
-      <c r="C46" s="5" t="n">
-        <v>174</v>
-      </c>
-      <c r="D46" s="6" t="n">
-        <v>19.99</v>
-      </c>
-      <c r="E46" s="4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="3" t="inlineStr">
-        <is>
-          <t>Weed Shop 3</t>
-        </is>
-      </c>
-      <c r="B47" s="4" t="n">
-        <v>0.9399999999999999</v>
-      </c>
-      <c r="C47" s="5" t="n">
-        <v>3304</v>
-      </c>
-      <c r="D47" s="6" t="n">
-        <v>19.5</v>
-      </c>
-      <c r="E47" s="4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="3" t="inlineStr">
-        <is>
-          <t>Wrench</t>
-        </is>
-      </c>
-      <c r="B48" s="4" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="C48" s="5" t="n">
-        <v>1024</v>
-      </c>
-      <c r="D48" s="6" t="n">
-        <v>24.99</v>
-      </c>
-      <c r="E48" s="4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="3" t="inlineStr">
-        <is>
-          <t>Hometopia</t>
-        </is>
-      </c>
-      <c r="B49" s="4" t="n">
-        <v>0.64</v>
-      </c>
-      <c r="C49" s="5" t="n">
-        <v>425</v>
-      </c>
-      <c r="D49" s="6" t="n">
-        <v>16.79</v>
-      </c>
-      <c r="E49" s="4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="3" t="inlineStr">
-        <is>
-          <t>Pool Cleaning Simulator</t>
-        </is>
-      </c>
-      <c r="B50" s="4" t="n">
-        <v>0.6899999999999999</v>
-      </c>
-      <c r="C50" s="5" t="n">
-        <v>173</v>
-      </c>
-      <c r="D50" s="6" t="n">
-        <v>11.79</v>
-      </c>
-      <c r="E50" s="4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1446,19 +1199,6 @@
     <hyperlink ref="A35" r:id="rId34"/>
     <hyperlink ref="A36" r:id="rId35"/>
     <hyperlink ref="A37" r:id="rId36"/>
-    <hyperlink ref="A38" r:id="rId37"/>
-    <hyperlink ref="A39" r:id="rId38"/>
-    <hyperlink ref="A40" r:id="rId39"/>
-    <hyperlink ref="A41" r:id="rId40"/>
-    <hyperlink ref="A42" r:id="rId41"/>
-    <hyperlink ref="A43" r:id="rId42"/>
-    <hyperlink ref="A44" r:id="rId43"/>
-    <hyperlink ref="A45" r:id="rId44"/>
-    <hyperlink ref="A46" r:id="rId45"/>
-    <hyperlink ref="A47" r:id="rId46"/>
-    <hyperlink ref="A48" r:id="rId47"/>
-    <hyperlink ref="A49" r:id="rId48"/>
-    <hyperlink ref="A50" r:id="rId49"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>